<commit_message>
add check balance, check mini statement, check custom statement
</commit_message>
<xml_diff>
--- a/Excels/CreateNewAccount.xlsx
+++ b/Excels/CreateNewAccount.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>customerID</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>accountID</t>
-  </si>
-  <si>
-    <t>Savings</t>
   </si>
 </sst>
 </file>
@@ -374,7 +371,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A3" sqref="A3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,42 +407,18 @@
       <c r="C2" s="1">
         <v>1000</v>
       </c>
-      <c r="D2"/>
+      <c r="D2">
+        <v>84915</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>90216</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1500</v>
-      </c>
       <c r="D3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>90216</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1000</v>
-      </c>
       <c r="D4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>90216</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1900</v>
-      </c>
+      <c r="C5" s="3"/>
       <c r="D5"/>
     </row>
   </sheetData>

</xml_diff>